<commit_message>
analyse update, designe, reseache, timesheet
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BL4CKD4G3R\Documents\BaWork\BaWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D79E31C-70EB-4D96-A45C-45155E1E9578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894E34CE-D10B-4883-9EF3-852B6B649404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A288747C-E72E-479A-AF89-6A8FE9B9D87D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Column7</t>
   </si>
@@ -112,6 +112,36 @@
   </si>
   <si>
     <t>17:00-19:00</t>
+  </si>
+  <si>
+    <t>00:00 - 03:00</t>
+  </si>
+  <si>
+    <t>aanpassen van Analyse van de Opdracht V</t>
+  </si>
+  <si>
+    <t>aanpassen analyse van de opdracht</t>
+  </si>
+  <si>
+    <t>aanpassen van rescearch en oplossingen</t>
+  </si>
+  <si>
+    <t>afwerken resaeach en oplossingen</t>
+  </si>
+  <si>
+    <t>verbeteren desgne van oplossing</t>
+  </si>
+  <si>
+    <t>16:00 - 17:00</t>
+  </si>
+  <si>
+    <t>feedback design van aanpak6 analyse opdracht</t>
+  </si>
+  <si>
+    <t>aanpassen research en ooplossingen</t>
+  </si>
+  <si>
+    <t>sedric, stefan</t>
   </si>
 </sst>
 </file>
@@ -175,8 +205,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22BACC80-893D-45E1-ACA1-5EC441836566}" name="Table1" displayName="Table1" ref="A5:G51" totalsRowShown="0">
-  <autoFilter ref="A5:G51" xr:uid="{61EDB86E-7F42-4853-AE10-96098250EB34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22BACC80-893D-45E1-ACA1-5EC441836566}" name="Table1" displayName="Table1" ref="A5:G52" totalsRowShown="0">
+  <autoFilter ref="A5:G52" xr:uid="{61EDB86E-7F42-4853-AE10-96098250EB34}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{80BB9B57-7B26-4E9F-B69A-79A631F8B111}" name="Datum"/>
     <tableColumn id="2" xr3:uid="{AE6C7809-9152-4CF0-95DF-C892A2B4512A}" name="Tijd"/>
@@ -487,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7507862-4D1F-4565-B4B3-362B04BEE18D}">
-  <dimension ref="A5:G15"/>
+  <dimension ref="A5:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,6 +699,85 @@
         <v>18</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43969</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43971</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43973</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>